<commit_message>
[GIPS] VerificationPackageGenerator upgraded to GS-Caliber 10-sheet format
- Replaced entire generate_calculation_workbook method
- Now creates 10 sheets with full formula transparency
- GS-Caliber colors: Navy, Gold, Green, Red
- All 15 metrics with Formula + Calculation + Result
- COMPREHENSIVE_TEST.py: 31/31 tests passing (100%)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/gips_outputs/Verification_Calculations_Composite.xlsx
+++ b/gips_outputs/Verification_Calculations_Composite.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2026-01-21 20:06:35</t>
+          <t>2026-01-21 20:21:16</t>
         </is>
       </c>
     </row>
@@ -3987,7 +3987,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2026-01-21 20:06:35</t>
+          <t>2026-01-21 20:21:16</t>
         </is>
       </c>
     </row>
@@ -4055,7 +4055,7 @@
         </is>
       </c>
       <c r="B11" s="13" t="n">
-        <v>0.2872876968326901</v>
+        <v>0.2872874093894</v>
       </c>
       <c r="C11" s="14" t="n">
         <v>0.2765609708573995</v>
@@ -4077,7 +4077,7 @@
         </is>
       </c>
       <c r="B12" s="13" t="n">
-        <v>-0.1817537751989279</v>
+        <v>-0.1817535281848931</v>
       </c>
       <c r="C12" s="14" t="n">
         <v>-0.0713999833188339</v>
@@ -4099,7 +4099,7 @@
         </is>
       </c>
       <c r="B13" s="13" t="n">
-        <v>0.2617581362475025</v>
+        <v>0.261757843743994</v>
       </c>
       <c r="C13" s="14" t="n">
         <v>0.1397451768677851</v>
@@ -4121,7 +4121,7 @@
         </is>
       </c>
       <c r="B14" s="13" t="n">
-        <v>0.2488645139506516</v>
+        <v>0.2488645961170239</v>
       </c>
       <c r="C14" s="14" t="n">
         <v>0.325641519707272</v>

</xml_diff>

<commit_message>
🔧 FIX: AI Hybrid Check API - correct GIPSRiskCalculator usage
Bug: GIPSRiskCalculator.__init__() takes 1-2 args but 3 were given
Root cause: API was calling calc = GIPSRiskCalculator(monthly_returns, benchmark_returns)
Fix:
- Initialize with just risk_free_rate: calc = GIPSRiskCalculator(risk_free_rate=0.04)
- Pass returns to each method: calc.calculate_volatility(returns)
- Use correct method names: calculate_var_historical() not calculate_var()

Tests: 31/31 PASS (100%)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/gips_outputs/Verification_Calculations_Composite.xlsx
+++ b/gips_outputs/Verification_Calculations_Composite.xlsx
@@ -640,7 +640,7 @@
     <row r="4">
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>Generated: 2026-01-21 20:42:19 | Portfolio: Composite | Periods: 61 months</t>
+          <t>Generated: 2026-01-21 20:59:14 | Portfolio: Composite | Periods: 61 months</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2026-01-21 20:42:19</t>
+          <t>2026-01-21 20:59:14</t>
         </is>
       </c>
     </row>
@@ -10558,14 +10558,14 @@
     <row r="10">
       <c r="B10" s="30" t="inlineStr">
         <is>
-          <t>Var(Benchmark) = 0.0041268574</t>
+          <t>Var(Benchmark) = 0.0041268572</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="26" t="inlineStr">
         <is>
-          <t>Beta = 0.0001123054 / 0.0041268574 = 0.027213</t>
+          <t>Beta = 0.0001123054 / 0.0041268572 = 0.027213</t>
         </is>
       </c>
     </row>

</xml_diff>